<commit_message>
vendors mobile banking correction
</commit_message>
<xml_diff>
--- a/00 Ü1 Anbieterevaluierung.xlsx
+++ b/00 Ü1 Anbieterevaluierung.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="153">
   <si>
     <t xml:space="preserve">Nr. </t>
   </si>
@@ -267,9 +267,6 @@
   </si>
   <si>
     <t>Paris</t>
-  </si>
-  <si>
-    <t>500-1000</t>
   </si>
   <si>
     <t>FIS</t>
@@ -897,10 +894,10 @@
   </sheetPr>
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C31" sqref="C31"/>
-      <selection pane="bottomLeft" activeCell="J15" sqref="J15"/>
+      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -988,8 +985,8 @@
       <c r="G2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>78</v>
+      <c r="H2" s="3">
+        <v>750</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>7</v>
@@ -1009,16 +1006,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" t="s">
         <v>80</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>81</v>
-      </c>
-      <c r="E3" t="s">
-        <v>82</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>7</v>
@@ -1027,7 +1024,7 @@
         <v>30000</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>7</v>
@@ -1047,16 +1044,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" t="s">
         <v>112</v>
-      </c>
-      <c r="D4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E4" t="s">
-        <v>113</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>7</v>
@@ -1065,7 +1062,7 @@
         <v>750</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>7</v>
@@ -1079,16 +1076,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D5" t="s">
         <v>51</v>
       </c>
       <c r="E5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>7</v>
@@ -1097,9 +1094,15 @@
         <v>21000</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="K5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L5" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1108,16 +1111,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>117</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>118</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>7</v>
@@ -1126,10 +1129,10 @@
         <v>160000</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>7</v>
@@ -1146,16 +1149,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>122</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>123</v>
       </c>
       <c r="D7" t="s">
         <v>51</v>
       </c>
       <c r="E7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>7</v>
@@ -1170,7 +1173,7 @@
         <v>7</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -1178,16 +1181,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>126</v>
       </c>
       <c r="D8" t="s">
         <v>51</v>
       </c>
       <c r="E8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>7</v>
@@ -1196,7 +1199,7 @@
         <v>2000</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>7</v>
@@ -1208,7 +1211,7 @@
         <v>7</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -1216,16 +1219,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D9" t="s">
         <v>130</v>
       </c>
-      <c r="D9" t="s">
-        <v>131</v>
-      </c>
       <c r="E9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>7</v>
@@ -1251,10 +1254,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>133</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>134</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
@@ -1269,7 +1272,7 @@
         <v>3800</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>7</v>
@@ -1289,16 +1292,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D11" t="s">
         <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>7</v>
@@ -1307,7 +1310,7 @@
         <v>5000</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>7</v>
@@ -1327,16 +1330,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>7</v>
@@ -1356,13 +1359,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="D13" t="s">
         <v>144</v>
-      </c>
-      <c r="D13" t="s">
-        <v>145</v>
       </c>
       <c r="E13" t="s">
         <v>13</v>
@@ -1391,16 +1394,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D14" t="s">
         <v>146</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="E14" t="s">
         <v>148</v>
-      </c>
-      <c r="D14" t="s">
-        <v>147</v>
-      </c>
-      <c r="E14" t="s">
-        <v>149</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>7</v>
@@ -1426,16 +1429,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>153</v>
-      </c>
       <c r="D15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>7</v>
@@ -1753,7 +1756,7 @@
         <v>42</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -1773,10 +1776,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -1796,10 +1799,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -1819,10 +1822,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>94</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -1842,10 +1845,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
@@ -1865,10 +1868,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
@@ -1885,10 +1888,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1908,16 +1911,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D9" t="s">
         <v>51</v>
       </c>
       <c r="E9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>7</v>
@@ -1928,10 +1931,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
@@ -1951,16 +1954,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D11" t="s">
         <v>51</v>
       </c>
       <c r="E11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>7</v>
@@ -1971,10 +1974,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>107</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>108</v>
       </c>
       <c r="D12" t="s">
         <v>10</v>
@@ -1991,16 +1994,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D13" t="s">
         <v>51</v>
       </c>
       <c r="E13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>7</v>
@@ -2011,10 +2014,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="D14" t="s">
         <v>10</v>

</xml_diff>